<commit_message>
updated figures, added R² calculation
</commit_message>
<xml_diff>
--- a/data/energy_measurements.xlsx
+++ b/data/energy_measurements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PatrickReisinger\git\impact_preproc_seizure_detection\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0E4311-D4A4-4179-BFAB-85165223DEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C71257-FF59-4B60-9A7E-090E942DDEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F0CE1263-D9CF-492E-A040-6DCF9A2C7114}"/>
+    <workbookView xWindow="41040" yWindow="4800" windowWidth="24690" windowHeight="14805" xr2:uid="{F0CE1263-D9CF-492E-A040-6DCF9A2C7114}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>model</t>
   </si>
@@ -47,9 +47,6 @@
     <t>adc_energy_75pct</t>
   </si>
   <si>
-    <t>cnn_energy_median</t>
-  </si>
-  <si>
     <t>adc_energy_median</t>
   </si>
   <si>
@@ -102,6 +99,21 @@
   </si>
   <si>
     <t>windows_8_0.0</t>
+  </si>
+  <si>
+    <t>cnn_energy_mean</t>
+  </si>
+  <si>
+    <t>cnn_energy_sec_mean</t>
+  </si>
+  <si>
+    <t>adc_energy_sec_median</t>
+  </si>
+  <si>
+    <t>adc_energy_sec_25pct</t>
+  </si>
+  <si>
+    <t>adc_energy_sec_75pct</t>
   </si>
 </sst>
 </file>
@@ -474,336 +486,543 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC5C71E-87BD-4017-A074-C330810060BE}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>49.15</v>
+      </c>
+      <c r="C2">
+        <v>49.15</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3.7888000000000002</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.85350399999999993</v>
+      </c>
+      <c r="F2" s="1">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1">
+        <v>3.7888000000000002</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.85350399999999993</v>
+      </c>
+      <c r="I2" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>49.1287066303193</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="B3">
+        <v>29.41</v>
+      </c>
+      <c r="C3">
+        <v>29.41</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1.8944000000000001</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.42675199999999996</v>
+      </c>
+      <c r="F3" s="1">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1.8944000000000001</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.42675199999999996</v>
+      </c>
+      <c r="I3" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>17.260000000000002</v>
+      </c>
+      <c r="C4">
+        <v>17.260000000000002</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.94720000000000004</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.21337599999999998</v>
+      </c>
+      <c r="F4" s="1">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.94720000000000004</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.21337599999999998</v>
+      </c>
+      <c r="I4" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>82.66</v>
+      </c>
+      <c r="C5">
+        <v>41.33</v>
+      </c>
+      <c r="D5" s="1">
+        <v>7.5776000000000003</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1.7070079999999999</v>
+      </c>
+      <c r="F5" s="1">
+        <v>32</v>
+      </c>
+      <c r="G5" s="1">
         <v>3.7888000000000002</v>
       </c>
-      <c r="D2" s="1">
+      <c r="H5" s="1">
         <v>0.85350399999999993</v>
       </c>
-      <c r="E2" s="1">
+      <c r="I5" s="1">
         <v>16</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>29.409887298010201</v>
-      </c>
-      <c r="C3" s="1">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>147.19999999999999</v>
+      </c>
+      <c r="C6">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="D6" s="1">
+        <v>15.155200000000001</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3.4140159999999997</v>
+      </c>
+      <c r="F6" s="1">
+        <v>64</v>
+      </c>
+      <c r="G6" s="1">
+        <v>3.7888000000000002</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.85350399999999993</v>
+      </c>
+      <c r="I6" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>731</v>
+      </c>
+      <c r="C7">
+        <v>91.34</v>
+      </c>
+      <c r="D7" s="1">
+        <v>30.310400000000001</v>
+      </c>
+      <c r="E7" s="1">
+        <v>6.8280319999999994</v>
+      </c>
+      <c r="F7" s="1">
+        <v>128</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3.7888000000000002</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.85350399999999993</v>
+      </c>
+      <c r="I7" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>49.45</v>
+      </c>
+      <c r="C8">
+        <v>49.45</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.60518400000000006</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.198656</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2.3951359999999999</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I8" s="1">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>49.49</v>
+      </c>
+      <c r="C9">
+        <v>49.49</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.19353599999999999</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.109568</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.54732799999999993</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>49.77</v>
+      </c>
+      <c r="C10">
+        <v>49.77</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.37119999999999997</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.17305599999999999</v>
+      </c>
+      <c r="F10" s="1">
+        <v>4.1292799999999996</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="I10" s="1">
+        <v>4.13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>49.39</v>
+      </c>
+      <c r="C11">
+        <v>49.39</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.27801599999999999</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.155136</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.40038400000000002</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>79.040000000000006</v>
+      </c>
+      <c r="C12">
+        <v>79.040000000000006</v>
+      </c>
+      <c r="D12" s="1">
+        <v>7.5776000000000003</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1.7070079999999999</v>
+      </c>
+      <c r="F12" s="1">
+        <v>32</v>
+      </c>
+      <c r="G12" s="1">
+        <v>7.58</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1.71</v>
+      </c>
+      <c r="I12" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>64.22</v>
+      </c>
+      <c r="C13">
+        <v>64.22</v>
+      </c>
+      <c r="D13" s="1">
+        <v>5.6832000000000003</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1.2802560000000001</v>
+      </c>
+      <c r="F13" s="1">
+        <v>24</v>
+      </c>
+      <c r="G13" s="1">
+        <v>5.68</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1.28</v>
+      </c>
+      <c r="I13" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>31.63</v>
+      </c>
+      <c r="C14">
+        <v>31.63</v>
+      </c>
+      <c r="D14" s="1">
         <v>1.8944000000000001</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E14" s="1">
         <v>0.42675199999999996</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F14" s="1">
         <v>8</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>17.261428222991501</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.94720000000000004</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.21337599999999998</v>
-      </c>
-      <c r="E4" s="1">
-        <v>4</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5">
-        <v>82.639121159911099</v>
-      </c>
-      <c r="C5" s="1">
-        <v>7.5776000000000003</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1.7070079999999999</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="G14" s="1">
+        <v>1.89</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="I14" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>49.19</v>
+      </c>
+      <c r="C15">
+        <v>98.39</v>
+      </c>
+      <c r="D15">
+        <v>3.79</v>
+      </c>
+      <c r="E15">
+        <v>0.85</v>
+      </c>
+      <c r="F15" s="1">
+        <v>16</v>
+      </c>
+      <c r="G15" s="1">
+        <v>7.58</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1.71</v>
+      </c>
+      <c r="I15" s="1">
         <v>32</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6">
-        <v>147.17487140372299</v>
-      </c>
-      <c r="C6" s="1">
-        <v>15.155200000000001</v>
-      </c>
-      <c r="D6" s="1">
-        <v>3.4140159999999997</v>
-      </c>
-      <c r="E6" s="1">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>82.4</v>
+      </c>
+      <c r="C16">
+        <v>82.39</v>
+      </c>
+      <c r="D16">
+        <v>7.58</v>
+      </c>
+      <c r="E16">
+        <v>1.71</v>
+      </c>
+      <c r="F16" s="1">
+        <v>32</v>
+      </c>
+      <c r="G16" s="1">
+        <v>7.58</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1.71</v>
+      </c>
+      <c r="I16" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>144.9</v>
+      </c>
+      <c r="C17">
+        <v>72.45</v>
+      </c>
+      <c r="D17">
+        <v>15.16</v>
+      </c>
+      <c r="E17">
+        <v>3.41</v>
+      </c>
+      <c r="F17" s="1">
         <v>64</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7">
-        <v>730.93048936128594</v>
-      </c>
-      <c r="C7" s="1">
-        <v>30.310400000000001</v>
-      </c>
-      <c r="D7" s="1">
-        <v>6.8280319999999994</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="G17" s="1">
+        <v>7.58</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1.71</v>
+      </c>
+      <c r="I17" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>730.9</v>
+      </c>
+      <c r="C18">
+        <v>182.73</v>
+      </c>
+      <c r="D18">
+        <v>30.31</v>
+      </c>
+      <c r="E18">
+        <v>6.83</v>
+      </c>
+      <c r="F18" s="1">
         <v>128</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>49.444706074893404</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.60518400000000006</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.198656</v>
-      </c>
-      <c r="E8" s="1">
-        <v>2.3951359999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>49.472581004723899</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.19353599999999999</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.109568</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.54732799999999993</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>49.756511401384998</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.37119999999999997</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.17305599999999999</v>
-      </c>
-      <c r="E10" s="1">
-        <v>4.1292799999999996</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>49.368155940435805</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0.27801599999999999</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.155136</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0.40038400000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>79.046362875960696</v>
-      </c>
-      <c r="C12" s="1">
-        <v>7.5776000000000003</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1.7070079999999999</v>
-      </c>
-      <c r="E12" s="1">
+      <c r="G18" s="1">
+        <v>7.58</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1.71</v>
+      </c>
+      <c r="I18" s="1">
         <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>64.189284576103006</v>
-      </c>
-      <c r="C13" s="1">
-        <v>5.6832000000000003</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1.2802560000000001</v>
-      </c>
-      <c r="E13" s="1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>31.631098941899801</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1.8944000000000001</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0.42675199999999996</v>
-      </c>
-      <c r="E14" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>49.165606250055099</v>
-      </c>
-      <c r="C15">
-        <v>3.7888000000000002</v>
-      </c>
-      <c r="D15">
-        <v>0.85350399999999993</v>
-      </c>
-      <c r="E15" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>82.415993530303197</v>
-      </c>
-      <c r="C16">
-        <v>7.5776000000000003</v>
-      </c>
-      <c r="D16">
-        <v>1.7070079999999999</v>
-      </c>
-      <c r="E16" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17">
-        <v>144.82426463905699</v>
-      </c>
-      <c r="C17">
-        <v>15.155200000000001</v>
-      </c>
-      <c r="D17">
-        <v>3.4140159999999997</v>
-      </c>
-      <c r="E17" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18">
-        <v>730.85865545459001</v>
-      </c>
-      <c r="C18">
-        <v>30.310400000000001</v>
-      </c>
-      <c r="D18">
-        <v>6.8280319999999994</v>
-      </c>
-      <c r="E18" s="1">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -813,15 +1032,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="042749b8-1cdb-4a39-88ba-a3a4758ca8b9" xsi:nil="true"/>
@@ -832,7 +1042,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100588D044A10F6A246B187C3B32D21720C" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3956ee0a2953ed6e730ceccad797a3ec">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="572143db-96f3-443e-a630-e59352fb5c9e" xmlns:ns3="042749b8-1cdb-4a39-88ba-a3a4758ca8b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b90bcca0d4edfb13b70b1c9100ab9bb9" ns2:_="" ns3:_="">
     <xsd:import namespace="572143db-96f3-443e-a630-e59352fb5c9e"/>
@@ -1087,15 +1297,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7308050-462B-48A4-A534-51FA85838F96}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC283E08-7777-4EF8-B5A3-A568437F7589}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1106,7 +1317,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DE37C00-76FD-4BBC-97D6-C6088C195A0C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1123,4 +1334,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7308050-462B-48A4-A534-51FA85838F96}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>